<commit_message>
Increase font size in Purchase Payment excel
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/purchasePayment.xlsx
+++ b/src/main/resources/excel/purchasePayment.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PJ\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PJ\git\magic\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C82FBEA-FE12-4AD5-9BD5-DFDB23BF6691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1D4989-0911-49B2-95C4-B382D915E649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{648E9802-BF24-4F6C-ABA9-DF84990602AA}"/>
   </bookViews>
@@ -44,7 +44,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="6"/>
+      <sz val="7"/>
       <color theme="1"/>
       <name val="Courier New"/>
       <family val="3"/>
@@ -392,11 +392,9 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="7.8" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="9.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="16384" width="8.88671875" style="1"/>
   </cols>

</xml_diff>

<commit_message>
Increase font size for Purchase Payment excel
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/purchasePayment.xlsx
+++ b/src/main/resources/excel/purchasePayment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PJ\git\magic\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1D4989-0911-49B2-95C4-B382D915E649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0833F22-D067-4061-854B-10DC7ECF0F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{648E9802-BF24-4F6C-ABA9-DF84990602AA}"/>
   </bookViews>
@@ -44,7 +44,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="7"/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Courier New"/>
       <family val="3"/>
@@ -394,7 +394,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="9.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="10.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="8.88671875" style="1"/>
   </cols>

</xml_diff>